<commit_message>
fixing typo in functions table
</commit_message>
<xml_diff>
--- a/inst/extdata/Functions.xlsx
+++ b/inst/extdata/Functions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/law145/Desktop/packages/dbGaPCheckup/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6536AC4D-4D9E-5241-BEC9-AA20C2FEC7D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A720976-5B8A-7E45-BF2A-806918F62FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39780" yWindow="2300" windowWidth="28040" windowHeight="16940" xr2:uid="{0EA5F04A-9331-CF41-B115-F8A4A1753AE3}"/>
   </bookViews>
@@ -215,9 +215,6 @@
     <t xml:space="preserve">Reorders the data dictionary to match the data set. </t>
   </si>
   <si>
-    <t>Updates the data dictionary so variable names match those listed in the data set.</t>
-  </si>
-  <si>
     <t>Adds additional fields required by this package including variable type ('TYPE'), minimum value ('MIN'), and maximum value ('MAX').</t>
   </si>
   <si>
@@ -246,6 +243,9 @@
   </si>
   <si>
     <t>Checks that the number of variables match between the data set and data dictionary.</t>
+  </si>
+  <si>
+    <t>Updates the data set so variable names match those listed in the data dictionary.</t>
   </si>
 </sst>
 </file>
@@ -293,14 +293,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -321,7 +320,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -609,7 +608,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -620,7 +619,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -674,7 +673,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -727,10 +726,10 @@
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -781,8 +780,8 @@
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>62</v>
+      <c r="C13" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -823,7 +822,7 @@
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -835,85 +834,85 @@
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>60</v>
+      <c r="C18" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>59</v>
+      <c r="C19" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D24" s="1"/>
@@ -943,14 +942,14 @@
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" s="1"/>
     </row>
@@ -991,10 +990,10 @@
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C31" s="2" t="s">

</xml_diff>

<commit_message>
Updates to id_check to flag rows with missing SUBJECT_ID
</commit_message>
<xml_diff>
--- a/inst/extdata/Functions.xlsx
+++ b/inst/extdata/Functions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/law145/Desktop/packages/dbGaPCheckup/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A720976-5B8A-7E45-BF2A-806918F62FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6375254-EFAB-7044-BEFC-74D6CCC4F970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39780" yWindow="2300" windowWidth="28040" windowHeight="16940" xr2:uid="{0EA5F04A-9331-CF41-B115-F8A4A1753AE3}"/>
   </bookViews>
@@ -176,9 +176,6 @@
     <t>Checks for dbGaP required fields: variable name (VARNAME), variable description (VARDESC), units (UNITS), and variable value and meaning (VALUES).</t>
   </si>
   <si>
-    <t xml:space="preserve">Checks that the first column of the data set is the primary ID for each participant labeled as SUBJECT_ID and that the values contain no spaces, padded zeros, or other illegal characters. </t>
-  </si>
-  <si>
     <t>Checks for NA values in the data set and, if NA values are present, also checks for an encoded NA value=meaning description.</t>
   </si>
   <si>
@@ -246,6 +243,9 @@
   </si>
   <si>
     <t>Updates the data set so variable names match those listed in the data dictionary.</t>
+  </si>
+  <si>
+    <t>Checks that the first column of the data set is the primary ID for each participant labeled as SUBJECT_ID, that values contain no illegal characters or padded zeros, and that each participant has an ID.</t>
   </si>
 </sst>
 </file>
@@ -320,7 +320,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -608,7 +608,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -619,7 +619,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,7 +673,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -697,7 +697,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -721,7 +721,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -745,7 +745,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -781,7 +781,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -805,7 +805,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -817,7 +817,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -829,79 +829,79 @@
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="C20" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -913,7 +913,7 @@
         <v>34</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -949,7 +949,7 @@
         <v>21</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D27" s="1"/>
     </row>
@@ -982,7 +982,7 @@
         <v>39</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>29</v>
@@ -994,7 +994,7 @@
         <v>40</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
update misc_format_check() to check that there are no missing VARNAME cells
</commit_message>
<xml_diff>
--- a/inst/extdata/Functions.xlsx
+++ b/inst/extdata/Functions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/law145/Desktop/packages/dbGaPCheckup/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728EFD23-9FE2-F04D-9769-53846687F8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D64A49-C543-8A43-80E3-E4961C1CA101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39780" yWindow="2300" windowWidth="28040" windowHeight="16940" xr2:uid="{0EA5F04A-9331-CF41-B115-F8A4A1753AE3}"/>
   </bookViews>
@@ -215,9 +215,6 @@
     <t xml:space="preserve">Checks for consistent usage of encoded values and missing value codes between the data dictionary and the data set. </t>
   </si>
   <si>
-    <t xml:space="preserve">Checks miscellaneous dbGaP formatting requirements to ensure (1) no duplicate variable names; (2) variable names do not contain "dbgap"; (3) there are no duplicate column names in the dictionary; and (4) column names falling after VALUES column are unnamed. </t>
-  </si>
-  <si>
     <t>reorder_data</t>
   </si>
   <si>
@@ -246,6 +243,9 @@
   </si>
   <si>
     <t xml:space="preserve">Checks for empty or duplicate rows in the data set and data dictionary. </t>
+  </si>
+  <si>
+    <t>Checks miscellaneous dbGaP formatting requirements to ensure (1) no empty variable names; (2) no duplicate variable names; (3) variable names do not contain "dbgap"; (4) there are no duplicate column names in the dictionary; and (5) column names falling after `VALUES` column are unnamed.</t>
   </si>
 </sst>
 </file>
@@ -619,7 +619,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,7 +673,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -697,7 +697,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -709,7 +709,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -781,7 +781,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -853,7 +853,7 @@
         <v>54</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -871,37 +871,37 @@
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23" s="1"/>
     </row>

</xml_diff>